<commit_message>
4.2 - correcciones en generacion de listado
</commit_message>
<xml_diff>
--- a/Resultados.xlsx
+++ b/Resultados.xlsx
@@ -1,22 +1,40 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25128"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/652fac3d04715f97/Proyecto Terminal/TerminalProject/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="43" documentId="11_4162231CA188538EF3A07DA6EC881050B57E7C22" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7C96747A-CEE9-405F-AD9C-B7E9B724AB67}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="STIF" sheetId="1" r:id="rId1"/>
     <sheet name="KNN" sheetId="2" r:id="rId2"/>
     <sheet name="Eigenfaces" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="50">
   <si>
     <t>Sujetos</t>
   </si>
@@ -163,14 +181,25 @@
   </si>
   <si>
     <t>Promedio</t>
+  </si>
+  <si>
+    <t>Promedio Geom</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -198,19 +227,28 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -252,7 +290,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -284,9 +322,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -318,6 +374,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -493,14 +567,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:H43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L33" sqref="L33"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -526,7 +602,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -534,45 +610,51 @@
         <v>1</v>
       </c>
       <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
         <v>0.5</v>
       </c>
-      <c r="D3">
+      <c r="E3">
         <v>0.3</v>
       </c>
-      <c r="E3">
-        <v>0.9</v>
-      </c>
       <c r="F3">
-        <v>0.7</v>
+        <v>0.9</v>
       </c>
       <c r="G3">
+        <v>0.7</v>
+      </c>
+      <c r="H3">
         <v>0.6</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>9</v>
       </c>
       <c r="B4">
-        <v>0.7</v>
+        <v>1</v>
       </c>
       <c r="C4">
-        <v>0.8</v>
+        <v>0.7</v>
       </c>
       <c r="D4">
+        <v>0.8</v>
+      </c>
+      <c r="E4">
         <v>0.3</v>
       </c>
-      <c r="E4">
-        <v>0.9</v>
-      </c>
       <c r="F4">
-        <v>0.7</v>
+        <v>0.9</v>
       </c>
       <c r="G4">
+        <v>0.7</v>
+      </c>
+      <c r="H4">
         <v>0.5</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -583,42 +665,48 @@
         <v>1</v>
       </c>
       <c r="D5">
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="E5">
-        <v>1</v>
+        <v>0.8</v>
       </c>
       <c r="F5">
-        <v>0.9</v>
+        <v>1</v>
       </c>
       <c r="G5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8">
+        <v>0.9</v>
+      </c>
+      <c r="H5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>11</v>
       </c>
       <c r="B6">
-        <v>1</v>
+        <v>0.9</v>
       </c>
       <c r="C6">
         <v>1</v>
       </c>
       <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="E6">
         <v>0.2</v>
       </c>
-      <c r="E6">
-        <v>0.8</v>
-      </c>
       <c r="F6">
-        <v>0.9</v>
+        <v>0.8</v>
       </c>
       <c r="G6">
         <v>0.9</v>
       </c>
-    </row>
-    <row r="7" spans="1:8">
+      <c r="H6">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -629,42 +717,48 @@
         <v>1</v>
       </c>
       <c r="D7">
+        <v>1</v>
+      </c>
+      <c r="E7">
         <v>0.5</v>
       </c>
-      <c r="E7">
-        <v>1</v>
-      </c>
       <c r="F7">
+        <v>1</v>
+      </c>
+      <c r="G7">
         <v>0.6</v>
       </c>
-      <c r="G7">
-        <v>0.9</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8">
+      <c r="H7">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>13</v>
       </c>
       <c r="B8">
-        <v>0.8</v>
+        <v>0.7</v>
       </c>
       <c r="C8">
+        <v>0.8</v>
+      </c>
+      <c r="D8">
         <v>0.6</v>
       </c>
-      <c r="D8">
-        <v>0.8</v>
-      </c>
       <c r="E8">
-        <v>0.7</v>
+        <v>0.8</v>
       </c>
       <c r="F8">
-        <v>0.8</v>
+        <v>0.7</v>
       </c>
       <c r="G8">
+        <v>0.8</v>
+      </c>
+      <c r="H8">
         <v>0.6</v>
       </c>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>14</v>
       </c>
@@ -675,162 +769,183 @@
         <v>1</v>
       </c>
       <c r="D9">
-        <v>0.9</v>
+        <v>1</v>
       </c>
       <c r="E9">
         <v>0.9</v>
       </c>
       <c r="F9">
-        <v>1</v>
+        <v>0.9</v>
       </c>
       <c r="G9">
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="1:8">
+      <c r="H9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>15</v>
       </c>
       <c r="B10">
-        <v>0.7</v>
+        <v>1</v>
       </c>
       <c r="C10">
-        <v>0.8</v>
+        <v>0.7</v>
       </c>
       <c r="D10">
+        <v>0.8</v>
+      </c>
+      <c r="E10">
         <v>0.2</v>
       </c>
-      <c r="E10">
-        <v>1</v>
-      </c>
       <c r="F10">
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="G10">
+        <v>0.8</v>
+      </c>
+      <c r="H10">
         <v>0.5</v>
       </c>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>16</v>
       </c>
       <c r="B11">
-        <v>0.8</v>
+        <v>0.7</v>
       </c>
       <c r="C11">
-        <v>0.9</v>
+        <v>0.8</v>
       </c>
       <c r="D11">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="E11">
-        <v>0.6</v>
+        <v>0</v>
       </c>
       <c r="F11">
         <v>0.6</v>
       </c>
       <c r="G11">
-        <v>0.7</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8">
+        <v>0.6</v>
+      </c>
+      <c r="H11">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>17</v>
       </c>
       <c r="B12">
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="C12">
         <v>0.8</v>
       </c>
       <c r="D12">
-        <v>0</v>
+        <v>0.8</v>
       </c>
       <c r="E12">
-        <v>0.7</v>
+        <v>0</v>
       </c>
       <c r="F12">
-        <v>1</v>
+        <v>0.7</v>
       </c>
       <c r="G12">
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8">
+        <v>1</v>
+      </c>
+      <c r="H12">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>18</v>
       </c>
       <c r="B13">
-        <v>0.9</v>
+        <v>1</v>
       </c>
       <c r="C13">
-        <v>1</v>
+        <v>0.9</v>
       </c>
       <c r="D13">
         <v>1</v>
       </c>
       <c r="E13">
-        <v>0.9</v>
+        <v>1</v>
       </c>
       <c r="F13">
-        <v>0.8</v>
+        <v>0.9</v>
       </c>
       <c r="G13">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8">
+        <v>0.8</v>
+      </c>
+      <c r="H13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>19</v>
       </c>
       <c r="B14">
-        <v>0.9</v>
+        <v>1</v>
       </c>
       <c r="C14">
-        <v>1</v>
+        <v>0.9</v>
       </c>
       <c r="D14">
+        <v>1</v>
+      </c>
+      <c r="E14">
         <v>0.6</v>
       </c>
-      <c r="E14">
-        <v>0.8</v>
-      </c>
       <c r="F14">
         <v>0.8</v>
       </c>
       <c r="G14">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8">
+        <v>0.8</v>
+      </c>
+      <c r="H14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>20</v>
       </c>
       <c r="B15">
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="C15">
-        <v>0.9</v>
+        <v>0.8</v>
       </c>
       <c r="D15">
+        <v>0.9</v>
+      </c>
+      <c r="E15">
         <v>0.6</v>
       </c>
-      <c r="E15">
-        <v>0.9</v>
-      </c>
       <c r="F15">
+        <v>0.9</v>
+      </c>
+      <c r="G15">
         <v>0.5</v>
       </c>
-      <c r="G15">
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8">
+      <c r="H15">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>21</v>
       </c>
       <c r="B16">
-        <v>0.9</v>
+        <v>1</v>
       </c>
       <c r="C16">
         <v>0.9</v>
@@ -839,7 +954,7 @@
         <v>0.9</v>
       </c>
       <c r="E16">
-        <v>1</v>
+        <v>0.9</v>
       </c>
       <c r="F16">
         <v>1</v>
@@ -847,31 +962,37 @@
       <c r="G16">
         <v>1</v>
       </c>
-    </row>
-    <row r="17" spans="1:7">
+      <c r="H16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>22</v>
       </c>
       <c r="B17">
-        <v>0.7</v>
+        <v>1</v>
       </c>
       <c r="C17">
-        <v>1</v>
+        <v>0.7</v>
       </c>
       <c r="D17">
+        <v>1</v>
+      </c>
+      <c r="E17">
         <v>0.3</v>
       </c>
-      <c r="E17">
-        <v>1</v>
-      </c>
       <c r="F17">
         <v>1</v>
       </c>
       <c r="G17">
-        <v>0.9</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7">
+        <v>1</v>
+      </c>
+      <c r="H17">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>23</v>
       </c>
@@ -882,42 +1003,48 @@
         <v>1</v>
       </c>
       <c r="D18">
+        <v>1</v>
+      </c>
+      <c r="E18">
         <v>0.6</v>
       </c>
-      <c r="E18">
-        <v>0.9</v>
-      </c>
       <c r="F18">
-        <v>1</v>
+        <v>0.9</v>
       </c>
       <c r="G18">
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7">
+        <v>1</v>
+      </c>
+      <c r="H18">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>24</v>
       </c>
       <c r="B19">
-        <v>0.9</v>
+        <v>1</v>
       </c>
       <c r="C19">
-        <v>0.8</v>
+        <v>0.9</v>
       </c>
       <c r="D19">
+        <v>0.8</v>
+      </c>
+      <c r="E19">
         <v>0.3</v>
       </c>
-      <c r="E19">
-        <v>1</v>
-      </c>
       <c r="F19">
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="G19">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7">
+        <v>0.8</v>
+      </c>
+      <c r="H19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>25</v>
       </c>
@@ -928,24 +1055,27 @@
         <v>1</v>
       </c>
       <c r="D20">
+        <v>1</v>
+      </c>
+      <c r="E20">
         <v>0.6</v>
       </c>
-      <c r="E20">
-        <v>0.8</v>
-      </c>
       <c r="F20">
-        <v>1</v>
+        <v>0.8</v>
       </c>
       <c r="G20">
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7">
+        <v>1</v>
+      </c>
+      <c r="H20">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>26</v>
       </c>
       <c r="B21">
-        <v>1</v>
+        <v>0.9</v>
       </c>
       <c r="C21">
         <v>1</v>
@@ -954,16 +1084,19 @@
         <v>1</v>
       </c>
       <c r="E21">
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="F21">
-        <v>1</v>
+        <v>0.8</v>
       </c>
       <c r="G21">
         <v>1</v>
       </c>
-    </row>
-    <row r="22" spans="1:7">
+      <c r="H21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>27</v>
       </c>
@@ -971,174 +1104,195 @@
         <v>1</v>
       </c>
       <c r="C22">
-        <v>0.9</v>
+        <v>1</v>
       </c>
       <c r="D22">
-        <v>0.8</v>
+        <v>0.9</v>
       </c>
       <c r="E22">
-        <v>1</v>
+        <v>0.8</v>
       </c>
       <c r="F22">
         <v>1</v>
       </c>
       <c r="G22">
-        <v>0.7</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7">
+        <v>1</v>
+      </c>
+      <c r="H22">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>28</v>
       </c>
       <c r="B23">
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="C23">
+        <v>0.8</v>
+      </c>
+      <c r="D23">
         <v>0.6</v>
       </c>
-      <c r="D23">
-        <v>0.7</v>
-      </c>
       <c r="E23">
-        <v>0.8</v>
+        <v>0.7</v>
       </c>
       <c r="F23">
-        <v>0.9</v>
+        <v>0.8</v>
       </c>
       <c r="G23">
+        <v>0.9</v>
+      </c>
+      <c r="H23">
         <v>0.6</v>
       </c>
     </row>
-    <row r="24" spans="1:7">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>29</v>
       </c>
       <c r="B24">
+        <v>0.9</v>
+      </c>
+      <c r="C24">
         <v>0.2</v>
       </c>
-      <c r="C24">
-        <v>1</v>
-      </c>
       <c r="D24">
         <v>1</v>
       </c>
       <c r="E24">
-        <v>0.9</v>
+        <v>1</v>
       </c>
       <c r="F24">
-        <v>0.7</v>
+        <v>0.9</v>
       </c>
       <c r="G24">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7">
+        <v>0.7</v>
+      </c>
+      <c r="H24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>30</v>
       </c>
       <c r="B25">
-        <v>0.7</v>
+        <v>1</v>
       </c>
       <c r="C25">
-        <v>0.9</v>
+        <v>0.7</v>
       </c>
       <c r="D25">
+        <v>0.9</v>
+      </c>
+      <c r="E25">
         <v>0.1</v>
       </c>
-      <c r="E25">
-        <v>0.8</v>
-      </c>
       <c r="F25">
-        <v>0.7</v>
+        <v>0.8</v>
       </c>
       <c r="G25">
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7">
+        <v>0.7</v>
+      </c>
+      <c r="H25">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>31</v>
       </c>
       <c r="B26">
-        <v>0.7</v>
+        <v>1</v>
       </c>
       <c r="C26">
-        <v>0.8</v>
+        <v>0.7</v>
       </c>
       <c r="D26">
+        <v>0.8</v>
+      </c>
+      <c r="E26">
         <v>0.2</v>
       </c>
-      <c r="E26">
-        <v>0.9</v>
-      </c>
       <c r="F26">
-        <v>1</v>
+        <v>0.9</v>
       </c>
       <c r="G26">
+        <v>1</v>
+      </c>
+      <c r="H26">
         <v>0.4</v>
       </c>
     </row>
-    <row r="27" spans="1:7">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>32</v>
       </c>
       <c r="B27">
+        <v>1</v>
+      </c>
+      <c r="C27">
         <v>0.6</v>
       </c>
-      <c r="C27">
-        <v>0.9</v>
-      </c>
       <c r="D27">
+        <v>0.9</v>
+      </c>
+      <c r="E27">
         <v>0.2</v>
       </c>
-      <c r="E27">
-        <v>1</v>
-      </c>
       <c r="F27">
-        <v>0.9</v>
+        <v>1</v>
       </c>
       <c r="G27">
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7">
+        <v>0.9</v>
+      </c>
+      <c r="H27">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>33</v>
       </c>
       <c r="B28">
-        <v>0.7</v>
+        <v>1</v>
       </c>
       <c r="C28">
-        <v>0.9</v>
+        <v>0.7</v>
       </c>
       <c r="D28">
+        <v>0.9</v>
+      </c>
+      <c r="E28">
         <v>0.6</v>
       </c>
-      <c r="E28">
-        <v>1</v>
-      </c>
       <c r="F28">
         <v>1</v>
       </c>
       <c r="G28">
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7">
+        <v>1</v>
+      </c>
+      <c r="H28">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>34</v>
       </c>
       <c r="B29">
-        <v>1</v>
+        <v>0.7</v>
       </c>
       <c r="C29">
         <v>1</v>
       </c>
       <c r="D29">
-        <v>0.7</v>
+        <v>1</v>
       </c>
       <c r="E29">
-        <v>1</v>
+        <v>0.7</v>
       </c>
       <c r="F29">
         <v>1</v>
@@ -1146,8 +1300,11 @@
       <c r="G29">
         <v>1</v>
       </c>
-    </row>
-    <row r="30" spans="1:7">
+      <c r="H29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>35</v>
       </c>
@@ -1158,134 +1315,152 @@
         <v>1</v>
       </c>
       <c r="D30">
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="E30">
-        <v>1</v>
+        <v>0.8</v>
       </c>
       <c r="F30">
         <v>1</v>
       </c>
       <c r="G30">
-        <v>0.9</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7">
+        <v>1</v>
+      </c>
+      <c r="H30">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>36</v>
       </c>
       <c r="B31">
-        <v>0.7</v>
+        <v>1</v>
       </c>
       <c r="C31">
-        <v>1</v>
+        <v>0.7</v>
       </c>
       <c r="D31">
+        <v>1</v>
+      </c>
+      <c r="E31">
         <v>0.5</v>
       </c>
-      <c r="E31">
-        <v>1</v>
-      </c>
       <c r="F31">
         <v>1</v>
       </c>
       <c r="G31">
         <v>1</v>
       </c>
-    </row>
-    <row r="32" spans="1:7">
+      <c r="H31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>37</v>
       </c>
       <c r="B32">
+        <v>1</v>
+      </c>
+      <c r="C32">
         <v>0.4</v>
-      </c>
-      <c r="C32">
-        <v>0.5</v>
       </c>
       <c r="D32">
         <v>0.5</v>
       </c>
       <c r="E32">
-        <v>0.9</v>
+        <v>0.5</v>
       </c>
       <c r="F32">
+        <v>0.9</v>
+      </c>
+      <c r="G32">
         <v>0.6</v>
       </c>
-      <c r="G32">
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7">
+      <c r="H32">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>38</v>
       </c>
       <c r="B33">
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="C33">
         <v>0.8</v>
       </c>
       <c r="D33">
+        <v>0.8</v>
+      </c>
+      <c r="E33">
         <v>0.3</v>
       </c>
-      <c r="E33">
-        <v>1</v>
-      </c>
       <c r="F33">
-        <v>0.7</v>
+        <v>1</v>
       </c>
       <c r="G33">
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7">
+        <v>0.7</v>
+      </c>
+      <c r="H33">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>39</v>
       </c>
       <c r="B34">
-        <v>0.9</v>
+        <v>1</v>
       </c>
       <c r="C34">
-        <v>1</v>
+        <v>0.9</v>
       </c>
       <c r="D34">
         <v>1</v>
       </c>
       <c r="E34">
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="F34">
         <v>0.8</v>
       </c>
       <c r="G34">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7">
+        <v>0.8</v>
+      </c>
+      <c r="H34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>40</v>
       </c>
       <c r="B35">
-        <v>0.7</v>
+        <v>0.9</v>
       </c>
       <c r="C35">
-        <v>0.3</v>
+        <v>0.7</v>
       </c>
       <c r="D35">
         <v>0.3</v>
       </c>
       <c r="E35">
-        <v>0.8</v>
+        <v>0.3</v>
       </c>
       <c r="F35">
-        <v>0.7</v>
+        <v>0.8</v>
       </c>
       <c r="G35">
+        <v>0.7</v>
+      </c>
+      <c r="H35">
         <v>0.4</v>
       </c>
     </row>
-    <row r="36" spans="1:7">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>41</v>
       </c>
@@ -1302,171 +1477,195 @@
         <v>1</v>
       </c>
       <c r="F36">
-        <v>0.9</v>
+        <v>1</v>
       </c>
       <c r="G36">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7">
+        <v>0.9</v>
+      </c>
+      <c r="H36">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>42</v>
       </c>
       <c r="B37">
-        <v>0.8</v>
+        <v>0.9</v>
       </c>
       <c r="C37">
-        <v>1</v>
+        <v>0.8</v>
       </c>
       <c r="D37">
+        <v>1</v>
+      </c>
+      <c r="E37">
         <v>0.1</v>
       </c>
-      <c r="E37">
-        <v>0.7</v>
-      </c>
       <c r="F37">
-        <v>1</v>
+        <v>0.7</v>
       </c>
       <c r="G37">
         <v>1</v>
       </c>
-    </row>
-    <row r="38" spans="1:7">
+      <c r="H37">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>43</v>
       </c>
       <c r="B38">
+        <v>1</v>
+      </c>
+      <c r="C38">
         <v>0.6</v>
       </c>
-      <c r="C38">
-        <v>0.8</v>
-      </c>
       <c r="D38">
-        <v>0.7</v>
+        <v>0.8</v>
       </c>
       <c r="E38">
-        <v>0.8</v>
+        <v>0.7</v>
       </c>
       <c r="F38">
-        <v>1</v>
+        <v>0.8</v>
       </c>
       <c r="G38">
+        <v>1</v>
+      </c>
+      <c r="H38">
         <v>0.6</v>
       </c>
     </row>
-    <row r="39" spans="1:7">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>44</v>
       </c>
       <c r="B39">
-        <v>0.9</v>
+        <v>1</v>
       </c>
       <c r="C39">
         <v>0.9</v>
       </c>
       <c r="D39">
-        <v>0.8</v>
+        <v>0.9</v>
       </c>
       <c r="E39">
-        <v>0.7</v>
+        <v>0.8</v>
       </c>
       <c r="F39">
-        <v>0.8</v>
+        <v>0.7</v>
       </c>
       <c r="G39">
         <v>0.8</v>
       </c>
-    </row>
-    <row r="40" spans="1:7">
+      <c r="H39">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>45</v>
       </c>
       <c r="B40">
+        <v>1</v>
+      </c>
+      <c r="C40">
         <v>0.5</v>
       </c>
-      <c r="C40">
-        <v>0.9</v>
-      </c>
       <c r="D40">
+        <v>0.9</v>
+      </c>
+      <c r="E40">
         <v>0.3</v>
       </c>
-      <c r="E40">
-        <v>1</v>
-      </c>
       <c r="F40">
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="G40">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7">
+        <v>0.8</v>
+      </c>
+      <c r="H40">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>46</v>
       </c>
       <c r="B41">
-        <v>0</v>
+        <v>0.7</v>
       </c>
       <c r="C41">
+        <v>0</v>
+      </c>
+      <c r="D41">
         <v>0.6</v>
       </c>
-      <c r="D41">
+      <c r="E41">
         <v>0.3</v>
       </c>
-      <c r="E41">
+      <c r="F41">
         <v>0.6</v>
       </c>
-      <c r="F41">
-        <v>0.8</v>
-      </c>
       <c r="G41">
-        <v>0.7</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7">
+        <v>0.8</v>
+      </c>
+      <c r="H41">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>47</v>
       </c>
       <c r="B42">
-        <v>0.9</v>
+        <v>1</v>
       </c>
       <c r="C42">
         <v>0.9</v>
       </c>
       <c r="D42">
+        <v>0.9</v>
+      </c>
+      <c r="E42">
         <v>0.3</v>
       </c>
-      <c r="E42">
-        <v>1</v>
-      </c>
       <c r="F42">
         <v>1</v>
       </c>
       <c r="G42">
         <v>1</v>
       </c>
-    </row>
-    <row r="43" spans="1:7">
+      <c r="H42">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>48</v>
       </c>
       <c r="B43">
-        <v>0.795</v>
+        <v>0.96750000000000003</v>
       </c>
       <c r="C43">
-        <v>0.8675</v>
+        <v>0.79500000000000004</v>
       </c>
       <c r="D43">
-        <v>0.5275</v>
+        <v>0.86750000000000005</v>
       </c>
       <c r="E43">
-        <v>0.8825</v>
+        <v>0.52749999999999997</v>
       </c>
       <c r="F43">
-        <v>0.855</v>
+        <v>0.88249999999999995</v>
       </c>
       <c r="G43">
-        <v>0.8225</v>
+        <v>0.85499999999999998</v>
+      </c>
+      <c r="H43">
+        <v>0.82250000000000001</v>
       </c>
     </row>
   </sheetData>
@@ -1475,14 +1674,19 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A2:H43"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A2:H46"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="B44" sqref="B44"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="11.85546875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -1508,12 +1712,12 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>8</v>
       </c>
       <c r="B3">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="C3">
         <v>0</v>
@@ -1530,13 +1734,16 @@
       <c r="G3">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:8">
+      <c r="H3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>9</v>
       </c>
       <c r="B4">
-        <v>0</v>
+        <v>0.7</v>
       </c>
       <c r="C4">
         <v>0</v>
@@ -1553,13 +1760,16 @@
       <c r="G4">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:8">
+      <c r="H4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>10</v>
       </c>
       <c r="B5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C5">
         <v>0</v>
@@ -1576,13 +1786,16 @@
       <c r="G5">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:8">
+      <c r="H5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>11</v>
       </c>
       <c r="B6">
-        <v>0</v>
+        <v>0.8</v>
       </c>
       <c r="C6">
         <v>0</v>
@@ -1591,21 +1804,24 @@
         <v>0</v>
       </c>
       <c r="E6">
-        <v>0.4</v>
+        <v>0</v>
       </c>
       <c r="F6">
         <v>0.4</v>
       </c>
       <c r="G6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8">
+        <v>0.4</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>12</v>
       </c>
       <c r="B7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C7">
         <v>0</v>
@@ -1622,36 +1838,42 @@
       <c r="G7">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:8">
+      <c r="H7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>13</v>
       </c>
       <c r="B8">
-        <v>0</v>
+        <v>0.7</v>
       </c>
       <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8">
         <v>0.6</v>
       </c>
-      <c r="D8">
-        <v>0.7</v>
-      </c>
       <c r="E8">
-        <v>0.8</v>
+        <v>0.7</v>
       </c>
       <c r="F8">
+        <v>0.8</v>
+      </c>
+      <c r="G8">
         <v>0.5</v>
       </c>
-      <c r="G8">
+      <c r="H8">
         <v>0.6</v>
       </c>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>14</v>
       </c>
       <c r="B9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C9">
         <v>0</v>
@@ -1668,13 +1890,16 @@
       <c r="G9">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:8">
+      <c r="H9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>15</v>
       </c>
       <c r="B10">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="C10">
         <v>0</v>
@@ -1691,13 +1916,16 @@
       <c r="G10">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:8">
+      <c r="H10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>16</v>
       </c>
       <c r="B11">
-        <v>0</v>
+        <v>0.7</v>
       </c>
       <c r="C11">
         <v>0</v>
@@ -1714,20 +1942,23 @@
       <c r="G11">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:8">
+      <c r="H11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>17</v>
       </c>
       <c r="B12">
-        <v>0</v>
+        <v>0.7</v>
       </c>
       <c r="C12">
+        <v>0</v>
+      </c>
+      <c r="D12">
         <v>0.3</v>
       </c>
-      <c r="D12">
-        <v>0</v>
-      </c>
       <c r="E12">
         <v>0</v>
       </c>
@@ -1735,15 +1966,18 @@
         <v>0</v>
       </c>
       <c r="G12">
+        <v>0</v>
+      </c>
+      <c r="H12">
         <v>0.6</v>
       </c>
     </row>
-    <row r="13" spans="1:8">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>18</v>
       </c>
       <c r="B13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C13">
         <v>0</v>
@@ -1760,13 +1994,16 @@
       <c r="G13">
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:8">
+      <c r="H13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>19</v>
       </c>
       <c r="B14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C14">
         <v>0</v>
@@ -1783,13 +2020,16 @@
       <c r="G14">
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:8">
+      <c r="H14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>20</v>
       </c>
       <c r="B15">
-        <v>0</v>
+        <v>0.8</v>
       </c>
       <c r="C15">
         <v>0</v>
@@ -1806,13 +2046,16 @@
       <c r="G15">
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="1:8">
+      <c r="H15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>21</v>
       </c>
       <c r="B16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C16">
         <v>0</v>
@@ -1829,13 +2072,16 @@
       <c r="G16">
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="1:7">
+      <c r="H16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>22</v>
       </c>
       <c r="B17">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C17">
         <v>0</v>
@@ -1852,13 +2098,16 @@
       <c r="G17">
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="1:7">
+      <c r="H17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>23</v>
       </c>
       <c r="B18">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C18">
         <v>0</v>
@@ -1875,13 +2124,16 @@
       <c r="G18">
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="1:7">
+      <c r="H18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>24</v>
       </c>
       <c r="B19">
-        <v>0</v>
+        <v>0.7</v>
       </c>
       <c r="C19">
         <v>0</v>
@@ -1898,13 +2150,16 @@
       <c r="G19">
         <v>0</v>
       </c>
-    </row>
-    <row r="20" spans="1:7">
+      <c r="H19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>25</v>
       </c>
       <c r="B20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C20">
         <v>0</v>
@@ -1921,13 +2176,16 @@
       <c r="G20">
         <v>0</v>
       </c>
-    </row>
-    <row r="21" spans="1:7">
+      <c r="H20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>26</v>
       </c>
       <c r="B21">
-        <v>0</v>
+        <v>0.8</v>
       </c>
       <c r="C21">
         <v>0</v>
@@ -1944,13 +2202,16 @@
       <c r="G21">
         <v>0</v>
       </c>
-    </row>
-    <row r="22" spans="1:7">
+      <c r="H21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>27</v>
       </c>
       <c r="B22">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C22">
         <v>0</v>
@@ -1967,13 +2228,16 @@
       <c r="G22">
         <v>0</v>
       </c>
-    </row>
-    <row r="23" spans="1:7">
+      <c r="H22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>28</v>
       </c>
       <c r="B23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C23">
         <v>0</v>
@@ -1990,13 +2254,16 @@
       <c r="G23">
         <v>0</v>
       </c>
-    </row>
-    <row r="24" spans="1:7">
+      <c r="H23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>29</v>
       </c>
       <c r="B24">
-        <v>0</v>
+        <v>0.8</v>
       </c>
       <c r="C24">
         <v>0</v>
@@ -2013,13 +2280,16 @@
       <c r="G24">
         <v>0</v>
       </c>
-    </row>
-    <row r="25" spans="1:7">
+      <c r="H24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>30</v>
       </c>
       <c r="B25">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C25">
         <v>0</v>
@@ -2036,13 +2306,16 @@
       <c r="G25">
         <v>0</v>
       </c>
-    </row>
-    <row r="26" spans="1:7">
+      <c r="H25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>31</v>
       </c>
       <c r="B26">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C26">
         <v>0</v>
@@ -2059,13 +2332,16 @@
       <c r="G26">
         <v>0</v>
       </c>
-    </row>
-    <row r="27" spans="1:7">
+      <c r="H26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>32</v>
       </c>
       <c r="B27">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C27">
         <v>0</v>
@@ -2082,13 +2358,16 @@
       <c r="G27">
         <v>0</v>
       </c>
-    </row>
-    <row r="28" spans="1:7">
+      <c r="H27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>33</v>
       </c>
       <c r="B28">
-        <v>0</v>
+        <v>0.7</v>
       </c>
       <c r="C28">
         <v>0</v>
@@ -2105,13 +2384,16 @@
       <c r="G28">
         <v>0</v>
       </c>
-    </row>
-    <row r="29" spans="1:7">
+      <c r="H28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>34</v>
       </c>
       <c r="B29">
-        <v>0</v>
+        <v>0.7</v>
       </c>
       <c r="C29">
         <v>0</v>
@@ -2128,13 +2410,16 @@
       <c r="G29">
         <v>0</v>
       </c>
-    </row>
-    <row r="30" spans="1:7">
+      <c r="H29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>35</v>
       </c>
       <c r="B30">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C30">
         <v>0</v>
@@ -2151,13 +2436,16 @@
       <c r="G30">
         <v>0</v>
       </c>
-    </row>
-    <row r="31" spans="1:7">
+      <c r="H30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>36</v>
       </c>
       <c r="B31">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C31">
         <v>0</v>
@@ -2174,59 +2462,68 @@
       <c r="G31">
         <v>0</v>
       </c>
-    </row>
-    <row r="32" spans="1:7">
+      <c r="H31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>37</v>
       </c>
       <c r="B32">
+        <v>1</v>
+      </c>
+      <c r="C32">
         <v>0.4</v>
       </c>
-      <c r="C32">
-        <v>0</v>
-      </c>
       <c r="D32">
         <v>0</v>
       </c>
       <c r="E32">
-        <v>0.9</v>
+        <v>0</v>
       </c>
       <c r="F32">
-        <v>0.8</v>
+        <v>0.9</v>
       </c>
       <c r="G32">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7">
+        <v>0.8</v>
+      </c>
+      <c r="H32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>38</v>
       </c>
       <c r="B33">
-        <v>0</v>
+        <v>0.8</v>
       </c>
       <c r="C33">
+        <v>0</v>
+      </c>
+      <c r="D33">
         <v>0.2</v>
       </c>
-      <c r="D33">
-        <v>0</v>
-      </c>
       <c r="E33">
+        <v>0</v>
+      </c>
+      <c r="F33">
         <v>0.1</v>
       </c>
-      <c r="F33">
-        <v>0</v>
-      </c>
       <c r="G33">
+        <v>0</v>
+      </c>
+      <c r="H33">
         <v>0.6</v>
       </c>
     </row>
-    <row r="34" spans="1:7">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>39</v>
       </c>
       <c r="B34">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C34">
         <v>0</v>
@@ -2243,13 +2540,16 @@
       <c r="G34">
         <v>0</v>
       </c>
-    </row>
-    <row r="35" spans="1:7">
+      <c r="H34">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>40</v>
       </c>
       <c r="B35">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="C35">
         <v>0</v>
@@ -2266,13 +2566,16 @@
       <c r="G35">
         <v>0</v>
       </c>
-    </row>
-    <row r="36" spans="1:7">
+      <c r="H35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>41</v>
       </c>
       <c r="B36">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C36">
         <v>0</v>
@@ -2289,13 +2592,16 @@
       <c r="G36">
         <v>0</v>
       </c>
-    </row>
-    <row r="37" spans="1:7">
+      <c r="H36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>42</v>
       </c>
       <c r="B37">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="C37">
         <v>0</v>
@@ -2312,13 +2618,16 @@
       <c r="G37">
         <v>0</v>
       </c>
-    </row>
-    <row r="38" spans="1:7">
+      <c r="H37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>43</v>
       </c>
       <c r="B38">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C38">
         <v>0</v>
@@ -2335,13 +2644,16 @@
       <c r="G38">
         <v>0</v>
       </c>
-    </row>
-    <row r="39" spans="1:7">
+      <c r="H38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>44</v>
       </c>
       <c r="B39">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="C39">
         <v>0</v>
@@ -2358,13 +2670,16 @@
       <c r="G39">
         <v>0</v>
       </c>
-    </row>
-    <row r="40" spans="1:7">
+      <c r="H39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>45</v>
       </c>
       <c r="B40">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C40">
         <v>0</v>
@@ -2381,13 +2696,16 @@
       <c r="G40">
         <v>0</v>
       </c>
-    </row>
-    <row r="41" spans="1:7">
+      <c r="H40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>46</v>
       </c>
       <c r="B41">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C41">
         <v>0</v>
@@ -2404,8 +2722,11 @@
       <c r="G41">
         <v>0</v>
       </c>
-    </row>
-    <row r="42" spans="1:7">
+      <c r="H41">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>47</v>
       </c>
@@ -2413,7 +2734,7 @@
         <v>0.8</v>
       </c>
       <c r="C42">
-        <v>0</v>
+        <v>0.8</v>
       </c>
       <c r="D42">
         <v>0</v>
@@ -2427,44 +2748,89 @@
       <c r="G42">
         <v>0</v>
       </c>
-    </row>
-    <row r="43" spans="1:7">
+      <c r="H42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>48</v>
       </c>
       <c r="B43">
+        <v>0.88749999999999996</v>
+      </c>
+      <c r="C43">
         <v>0.03</v>
       </c>
-      <c r="C43">
-        <v>0.0275</v>
-      </c>
       <c r="D43">
-        <v>0.0175</v>
+        <v>2.75E-2</v>
       </c>
       <c r="E43">
-        <v>0.055</v>
+        <v>1.7500000000000002E-2</v>
       </c>
       <c r="F43">
-        <v>0.0425</v>
+        <v>5.5E-2</v>
       </c>
       <c r="G43">
-        <v>0.045</v>
-      </c>
+        <v>4.2500000000000003E-2</v>
+      </c>
+      <c r="H43">
+        <v>4.4999999999999998E-2</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>49</v>
+      </c>
+      <c r="B44">
+        <f>GEOMEAN(B3:B42)</f>
+        <v>0.89667687322203826</v>
+      </c>
+      <c r="C44" t="e">
+        <f>GEOMEAN(C3:C42)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="D44" t="e">
+        <f t="shared" ref="C44:H44" si="0">GEOMEAN(D3:D42)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="E44" t="e">
+        <f t="shared" si="0"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="F44" t="e">
+        <f t="shared" si="0"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="G44" t="e">
+        <f t="shared" si="0"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="H44" t="e">
+        <f t="shared" si="0"/>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D46" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A2:H43"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="H31" sqref="H31"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -2490,7 +2856,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -2513,7 +2879,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -2536,7 +2902,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -2559,7 +2925,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -2582,7 +2948,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -2605,7 +2971,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>13</v>
       </c>
@@ -2628,7 +2994,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>14</v>
       </c>
@@ -2651,7 +3017,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>15</v>
       </c>
@@ -2674,7 +3040,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>16</v>
       </c>
@@ -2697,7 +3063,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>17</v>
       </c>
@@ -2720,7 +3086,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:8">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>18</v>
       </c>
@@ -2743,7 +3109,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="14" spans="1:8">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>19</v>
       </c>
@@ -2766,7 +3132,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:8">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>20</v>
       </c>
@@ -2789,7 +3155,7 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="16" spans="1:8">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>21</v>
       </c>
@@ -2812,7 +3178,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:7">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>22</v>
       </c>
@@ -2835,7 +3201,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="18" spans="1:7">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>23</v>
       </c>
@@ -2858,7 +3224,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="19" spans="1:7">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>24</v>
       </c>
@@ -2881,7 +3247,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="20" spans="1:7">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>25</v>
       </c>
@@ -2904,7 +3270,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="21" spans="1:7">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>26</v>
       </c>
@@ -2927,7 +3293,7 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="22" spans="1:7">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>27</v>
       </c>
@@ -2950,7 +3316,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="23" spans="1:7">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>28</v>
       </c>
@@ -2973,7 +3339,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:7">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>29</v>
       </c>
@@ -2996,7 +3362,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="25" spans="1:7">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>30</v>
       </c>
@@ -3019,7 +3385,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:7">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>31</v>
       </c>
@@ -3042,7 +3408,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:7">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>32</v>
       </c>
@@ -3065,7 +3431,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:7">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>33</v>
       </c>
@@ -3088,7 +3454,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:7">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>34</v>
       </c>
@@ -3111,7 +3477,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="30" spans="1:7">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>35</v>
       </c>
@@ -3134,7 +3500,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:7">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>36</v>
       </c>
@@ -3157,7 +3523,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:7">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>37</v>
       </c>
@@ -3180,7 +3546,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:7">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>38</v>
       </c>
@@ -3203,7 +3569,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="34" spans="1:7">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>39</v>
       </c>
@@ -3226,7 +3592,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="35" spans="1:7">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>40</v>
       </c>
@@ -3249,7 +3615,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="36" spans="1:7">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>41</v>
       </c>
@@ -3272,7 +3638,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:7">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>42</v>
       </c>
@@ -3295,7 +3661,7 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="38" spans="1:7">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>43</v>
       </c>
@@ -3318,7 +3684,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="39" spans="1:7">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>44</v>
       </c>
@@ -3341,7 +3707,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="40" spans="1:7">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>45</v>
       </c>
@@ -3364,7 +3730,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="41" spans="1:7">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>46</v>
       </c>
@@ -3387,7 +3753,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="42" spans="1:7">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>47</v>
       </c>
@@ -3410,27 +3776,27 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:7">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>48</v>
       </c>
       <c r="B43">
-        <v>0.9875</v>
+        <v>0.98750000000000004</v>
       </c>
       <c r="C43">
-        <v>0.9025</v>
+        <v>0.90249999999999997</v>
       </c>
       <c r="D43">
         <v>0.3</v>
       </c>
       <c r="E43">
-        <v>0.0825</v>
+        <v>8.2500000000000004E-2</v>
       </c>
       <c r="F43">
         <v>0.86</v>
       </c>
       <c r="G43">
-        <v>0.7875</v>
+        <v>0.78749999999999998</v>
       </c>
     </row>
   </sheetData>

</xml_diff>